<commit_message>
Versão Final e homologada
Versão final e homologda pela area de negocios!
</commit_message>
<xml_diff>
--- a/Bases_xlsx/Base_baixa.xlsx
+++ b/Bases_xlsx/Base_baixa.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02.GIT_REPOSITORY\R_FATMAN_J1\01_R_FATMAN_J1\Bases_xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02.GIT_REPOSITORY\R_FATMAN_J1\01R_FATMAN_J1\R_FATMAN_J1\Bases_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050E169B-BBCD-45FB-B122-2F1D61EB4D1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BF4EBE-99A0-4C35-BAF2-3CDA0BF5A0DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
   <si>
     <t>Ctg nota fiscal</t>
   </si>
@@ -103,21 +102,12 @@
     <t>IPI3</t>
   </si>
   <si>
-    <t>Montante Basico</t>
-  </si>
-  <si>
-    <t>Taxa Imposto</t>
-  </si>
-  <si>
     <t>Outra base</t>
   </si>
   <si>
     <t>Emissão com base a nota fiscal xxxx Nestlé</t>
   </si>
   <si>
-    <t>Cód. Status</t>
-  </si>
-  <si>
     <t>1.57</t>
   </si>
   <si>
@@ -137,6 +127,36 @@
   </si>
   <si>
     <t>ICM3</t>
+  </si>
+  <si>
+    <t>Tipo Imposto_03</t>
+  </si>
+  <si>
+    <t>ICS3</t>
+  </si>
+  <si>
+    <t>Taxa Imposto_0102</t>
+  </si>
+  <si>
+    <t>Taxa Imposto_03</t>
+  </si>
+  <si>
+    <t>STG</t>
+  </si>
+  <si>
+    <t>Montante Basico_ICM3</t>
+  </si>
+  <si>
+    <t>Montante Basico_ICS3</t>
+  </si>
+  <si>
+    <t>Calculo_ICM3</t>
+  </si>
+  <si>
+    <t>Cod_status</t>
+  </si>
+  <si>
+    <t>Calculo_ICS3</t>
   </si>
 </sst>
 </file>
@@ -174,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,14 +217,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -220,99 +253,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>106645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>227047</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>162843</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6610350" y="2964145"/>
-          <a:ext cx="7637497" cy="3104198"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>520582</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>218356</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>28093</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6616582" y="6267450"/>
-          <a:ext cx="5184174" cy="3476143"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -578,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,21 +537,25 @@
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="39.42578125" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="39.42578125" customWidth="1"/>
+    <col min="26" max="26" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -653,31 +597,46 @@
         <v>19</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="Y1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -706,13 +665,13 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>16</v>
@@ -724,27 +683,42 @@
         <v>20</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="1">
         <v>1.57</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
+        <v>1.84</v>
+      </c>
+      <c r="U2" s="1">
+        <v>12</v>
+      </c>
+      <c r="V2" s="1">
         <v>18</v>
       </c>
-      <c r="T2" s="1">
+      <c r="W2" s="1">
         <v>1.57</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
+      <c r="X2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>0.14000000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -773,7 +747,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>12</v>
@@ -791,27 +765,40 @@
         <v>20</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="1"/>
+      <c r="S3" s="1">
         <v>1.57</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
         <v>18</v>
       </c>
-      <c r="T3" s="1">
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
         <v>1.57</v>
       </c>
-      <c r="U3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
+      <c r="X3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -840,13 +827,13 @@
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>16</v>
@@ -858,27 +845,42 @@
         <v>20</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" s="1">
         <v>1.57</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
+        <v>1.84</v>
+      </c>
+      <c r="U4" s="1">
+        <v>12</v>
+      </c>
+      <c r="V4" s="1">
         <v>18</v>
       </c>
-      <c r="T4" s="1">
+      <c r="W4" s="1">
         <v>1.57</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
+      <c r="X4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>0.14000000000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -907,7 +909,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>12</v>
@@ -925,43 +927,41 @@
         <v>20</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="1"/>
+      <c r="S5" s="1">
         <v>1.57</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T5" s="3">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
         <v>18</v>
       </c>
-      <c r="T5" s="1">
+      <c r="V5" s="1">
+        <v>0</v>
+      </c>
+      <c r="W5" s="1">
         <v>1.57</v>
       </c>
-      <c r="U5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
+      <c r="X5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>